<commit_message>
rearrange code in handleData
</commit_message>
<xml_diff>
--- a/handleData/data/regions.xlsx
+++ b/handleData/data/regions.xlsx
@@ -88,9 +88,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="m/d;@"/>
   </numFmts>
   <fonts count="24">
@@ -131,29 +131,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -167,7 +153,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -175,7 +161,29 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -189,22 +197,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -213,32 +205,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -253,10 +230,18 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -269,6 +254,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -289,13 +289,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -313,13 +319,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,19 +337,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -355,7 +367,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -367,7 +397,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -379,61 +427,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -451,19 +445,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -507,21 +507,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -539,11 +524,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -560,17 +558,19 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -585,7 +585,7 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -594,133 +594,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1366,10 +1366,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C132"/>
+  <dimension ref="A1:C131"/>
   <sheetViews>
     <sheetView topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="F122" sqref="F122"/>
+      <selection activeCell="A132" sqref="$A132:$XFD132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -2804,14 +2804,15 @@
         <v>91148</v>
       </c>
     </row>
-    <row r="131" spans="1:1">
+    <row r="131" spans="1:3">
       <c r="A131" s="5">
         <v>43990</v>
       </c>
-    </row>
-    <row r="132" spans="1:1">
-      <c r="A132" s="5">
-        <v>43991</v>
+      <c r="B131">
+        <v>117929</v>
+      </c>
+      <c r="C131">
+        <v>49427</v>
       </c>
     </row>
   </sheetData>
@@ -2823,10 +2824,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C130"/>
+  <dimension ref="A1:C131"/>
   <sheetViews>
-    <sheetView topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="A126" sqref="A126:A130"/>
+    <sheetView topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="A130" sqref="A130:A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -4247,6 +4248,17 @@
       </c>
       <c r="C130">
         <v>3138</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" s="5">
+        <v>43990</v>
+      </c>
+      <c r="B131">
+        <v>6508</v>
+      </c>
+      <c r="C131">
+        <v>1590</v>
       </c>
     </row>
   </sheetData>
@@ -4261,7 +4273,7 @@
   <dimension ref="A1:C131"/>
   <sheetViews>
     <sheetView topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="A126" sqref="A126:A131"/>
+      <selection activeCell="F123" sqref="F123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -5687,9 +5699,15 @@
         <v>16760</v>
       </c>
     </row>
-    <row r="131" spans="1:1">
+    <row r="131" spans="1:3">
       <c r="A131" s="5">
         <v>43990</v>
+      </c>
+      <c r="B131">
+        <v>27525</v>
+      </c>
+      <c r="C131">
+        <v>12795</v>
       </c>
     </row>
   </sheetData>
@@ -5701,10 +5719,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C130"/>
+  <dimension ref="A1:C131"/>
   <sheetViews>
     <sheetView topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="A124" sqref="A124:A130"/>
+      <selection activeCell="B131" sqref="B131:C131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -7127,6 +7145,17 @@
         <v>33988</v>
       </c>
     </row>
+    <row r="131" spans="1:3">
+      <c r="A131" s="5">
+        <v>43990</v>
+      </c>
+      <c r="B131">
+        <v>46386</v>
+      </c>
+      <c r="C131">
+        <v>26269</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -7136,10 +7165,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L132"/>
+  <dimension ref="A1:L131"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="C127" sqref="C127"/>
+      <selection activeCell="A131" sqref="$A131:$XFD131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14"/>
@@ -12058,14 +12087,42 @@
         <v>263</v>
       </c>
     </row>
-    <row r="131" spans="1:1">
+    <row r="131" spans="1:12">
       <c r="A131" s="5">
         <v>43990</v>
       </c>
-    </row>
-    <row r="132" spans="1:1">
-      <c r="A132" s="5">
-        <v>43991</v>
+      <c r="B131">
+        <v>68143</v>
+      </c>
+      <c r="C131">
+        <v>19947</v>
+      </c>
+      <c r="D131" s="5">
+        <v>43990</v>
+      </c>
+      <c r="E131">
+        <v>28543</v>
+      </c>
+      <c r="F131">
+        <v>17788</v>
+      </c>
+      <c r="G131" s="5">
+        <v>43990</v>
+      </c>
+      <c r="H131">
+        <v>19450</v>
+      </c>
+      <c r="I131">
+        <v>10993</v>
+      </c>
+      <c r="J131" s="5">
+        <v>43990</v>
+      </c>
+      <c r="K131">
+        <v>274</v>
+      </c>
+      <c r="L131">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix a bug in mkdir tmp
</commit_message>
<xml_diff>
--- a/handleData/data/regions.xlsx
+++ b/handleData/data/regions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16950" windowHeight="7290" activeTab="4"/>
+    <workbookView windowWidth="13030" windowHeight="7290" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="全球" sheetId="2" r:id="rId1"/>
@@ -87,10 +87,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="m/d;@"/>
   </numFmts>
   <fonts count="24">
@@ -131,7 +131,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -152,6 +152,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -159,9 +160,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -174,16 +174,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -198,18 +214,48 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -221,54 +267,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -283,7 +283,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -295,13 +337,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -313,157 +445,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -477,17 +477,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -507,17 +503,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -527,6 +532,15 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -546,31 +560,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -582,10 +582,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -594,16 +594,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -612,115 +612,115 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1366,10 +1366,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C131"/>
+  <dimension ref="A1:C138"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="A132" sqref="$A132:$XFD132"/>
+    <sheetView topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="D139" sqref="D139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -2815,6 +2815,77 @@
         <v>49427</v>
       </c>
     </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="5">
+        <v>43991</v>
+      </c>
+      <c r="B132">
+        <v>103210</v>
+      </c>
+      <c r="C132">
+        <v>53315</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="5">
+        <v>43992</v>
+      </c>
+      <c r="B133">
+        <v>135778</v>
+      </c>
+      <c r="C133">
+        <v>87908</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="5">
+        <v>43993</v>
+      </c>
+      <c r="B134">
+        <v>133774</v>
+      </c>
+      <c r="C134">
+        <v>128318</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" s="5">
+        <v>43994</v>
+      </c>
+      <c r="B135">
+        <v>137551</v>
+      </c>
+      <c r="C135">
+        <v>111174</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" s="5">
+        <v>43995</v>
+      </c>
+      <c r="B136">
+        <v>137665</v>
+      </c>
+      <c r="C136">
+        <v>76075</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" s="5">
+        <v>43996</v>
+      </c>
+      <c r="B137">
+        <v>136650</v>
+      </c>
+      <c r="C137">
+        <v>108403</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" s="5">
+        <v>43997</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -2824,10 +2895,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C131"/>
+  <dimension ref="A1:C138"/>
   <sheetViews>
-    <sheetView topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="A130" sqref="A130:A131"/>
+    <sheetView topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="H129" sqref="H129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -4261,6 +4332,77 @@
         <v>1590</v>
       </c>
     </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="5">
+        <v>43991</v>
+      </c>
+      <c r="B132">
+        <v>6667</v>
+      </c>
+      <c r="C132">
+        <v>3173</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="5">
+        <v>43992</v>
+      </c>
+      <c r="B133">
+        <v>5867</v>
+      </c>
+      <c r="C133">
+        <v>4499</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="5">
+        <v>43993</v>
+      </c>
+      <c r="B134">
+        <v>6999</v>
+      </c>
+      <c r="C134">
+        <v>4353</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" s="5">
+        <v>43994</v>
+      </c>
+      <c r="B135">
+        <v>6872</v>
+      </c>
+      <c r="C135">
+        <v>3424</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" s="5">
+        <v>43995</v>
+      </c>
+      <c r="B136">
+        <v>8331</v>
+      </c>
+      <c r="C136">
+        <v>3967</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" s="5">
+        <v>43996</v>
+      </c>
+      <c r="B137">
+        <v>8323</v>
+      </c>
+      <c r="C137">
+        <v>4058</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" s="5">
+        <v>43997</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -4270,10 +4412,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C131"/>
+  <dimension ref="A1:C138"/>
   <sheetViews>
     <sheetView topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="F123" sqref="F123"/>
+      <selection activeCell="B132" sqref="B132:C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -5710,6 +5852,77 @@
         <v>12795</v>
       </c>
     </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="5">
+        <v>43991</v>
+      </c>
+      <c r="B132">
+        <v>24858</v>
+      </c>
+      <c r="C132">
+        <v>11151</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="5">
+        <v>43992</v>
+      </c>
+      <c r="B133">
+        <v>26323</v>
+      </c>
+      <c r="C133">
+        <v>20214</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="5">
+        <v>43993</v>
+      </c>
+      <c r="B134">
+        <v>28235</v>
+      </c>
+      <c r="C134">
+        <v>20026</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" s="5">
+        <v>43994</v>
+      </c>
+      <c r="B135">
+        <v>28684</v>
+      </c>
+      <c r="C135">
+        <v>18366</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" s="5">
+        <v>43995</v>
+      </c>
+      <c r="B136">
+        <v>30141</v>
+      </c>
+      <c r="C136">
+        <v>19416</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" s="5">
+        <v>43996</v>
+      </c>
+      <c r="B137">
+        <v>30305</v>
+      </c>
+      <c r="C137">
+        <v>24783</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" s="5">
+        <v>43997</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -5719,10 +5932,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C131"/>
+  <dimension ref="A1:C138"/>
   <sheetViews>
-    <sheetView topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="B131" sqref="B131:C131"/>
+    <sheetView topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="B132" sqref="B132:C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -7156,6 +7369,77 @@
         <v>26269</v>
       </c>
     </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="5">
+        <v>43991</v>
+      </c>
+      <c r="B132">
+        <v>42718</v>
+      </c>
+      <c r="C132">
+        <v>25531</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="5">
+        <v>43992</v>
+      </c>
+      <c r="B133">
+        <v>44106</v>
+      </c>
+      <c r="C133">
+        <v>34875</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="5">
+        <v>43993</v>
+      </c>
+      <c r="B134">
+        <v>47087</v>
+      </c>
+      <c r="C134">
+        <v>34790</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" s="5">
+        <v>43994</v>
+      </c>
+      <c r="B135">
+        <v>49210</v>
+      </c>
+      <c r="C135">
+        <v>36097</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" s="5">
+        <v>43995</v>
+      </c>
+      <c r="B136">
+        <v>51098</v>
+      </c>
+      <c r="C136">
+        <v>32734</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" s="5">
+        <v>43996</v>
+      </c>
+      <c r="B137">
+        <v>50635</v>
+      </c>
+      <c r="C137">
+        <v>38704</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" s="5">
+        <v>43997</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -7165,10 +7449,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L131"/>
+  <dimension ref="A1:L138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="A131" sqref="$A131:$XFD131"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="E93" sqref="E93:E137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14"/>
@@ -12123,6 +12407,239 @@
       </c>
       <c r="L131">
         <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12">
+      <c r="A132" s="5">
+        <v>43991</v>
+      </c>
+      <c r="B132">
+        <v>57055</v>
+      </c>
+      <c r="C132">
+        <v>22134</v>
+      </c>
+      <c r="D132" s="5">
+        <v>43991</v>
+      </c>
+      <c r="E132">
+        <v>25853</v>
+      </c>
+      <c r="F132">
+        <v>21701</v>
+      </c>
+      <c r="G132" s="5">
+        <v>43991</v>
+      </c>
+      <c r="H132">
+        <v>18484</v>
+      </c>
+      <c r="I132">
+        <v>8359</v>
+      </c>
+      <c r="J132" s="5">
+        <v>43991</v>
+      </c>
+      <c r="K132">
+        <v>342</v>
+      </c>
+      <c r="L132">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12">
+      <c r="A133" s="5">
+        <v>43992</v>
+      </c>
+      <c r="B133">
+        <v>88184</v>
+      </c>
+      <c r="C133">
+        <v>47481</v>
+      </c>
+      <c r="D133" s="5">
+        <v>43992</v>
+      </c>
+      <c r="E133">
+        <v>27776</v>
+      </c>
+      <c r="F133">
+        <v>22117</v>
+      </c>
+      <c r="G133" s="5">
+        <v>43992</v>
+      </c>
+      <c r="H133">
+        <v>18004</v>
+      </c>
+      <c r="I133">
+        <v>17353</v>
+      </c>
+      <c r="J133" s="5">
+        <v>43992</v>
+      </c>
+      <c r="K133">
+        <v>281</v>
+      </c>
+      <c r="L133">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12">
+      <c r="A134" s="5">
+        <v>43993</v>
+      </c>
+      <c r="B134">
+        <v>83304</v>
+      </c>
+      <c r="C134">
+        <v>82189</v>
+      </c>
+      <c r="D134" s="5">
+        <v>43993</v>
+      </c>
+      <c r="E134">
+        <v>29187</v>
+      </c>
+      <c r="F134">
+        <v>25984</v>
+      </c>
+      <c r="G134" s="5">
+        <v>43993</v>
+      </c>
+      <c r="H134">
+        <v>19660</v>
+      </c>
+      <c r="I134">
+        <v>18545</v>
+      </c>
+      <c r="J134" s="5">
+        <v>43993</v>
+      </c>
+      <c r="K134">
+        <v>344</v>
+      </c>
+      <c r="L134">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12">
+      <c r="A135" s="5">
+        <v>43994</v>
+      </c>
+      <c r="B135">
+        <v>83887</v>
+      </c>
+      <c r="C135">
+        <v>73394</v>
+      </c>
+      <c r="D135" s="5">
+        <v>43994</v>
+      </c>
+      <c r="E135">
+        <v>32975</v>
+      </c>
+      <c r="F135">
+        <v>20174</v>
+      </c>
+      <c r="G135" s="5">
+        <v>43994</v>
+      </c>
+      <c r="H135">
+        <v>18800</v>
+      </c>
+      <c r="I135">
+        <v>16074</v>
+      </c>
+      <c r="J135" s="5">
+        <v>43994</v>
+      </c>
+      <c r="K135">
+        <v>433</v>
+      </c>
+      <c r="L135">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12">
+      <c r="A136" s="5">
+        <v>43995</v>
+      </c>
+      <c r="B136">
+        <v>77028</v>
+      </c>
+      <c r="C136">
+        <v>28133</v>
+      </c>
+      <c r="D136" s="5">
+        <v>43995</v>
+      </c>
+      <c r="E136">
+        <v>37336</v>
+      </c>
+      <c r="F136">
+        <v>31351</v>
+      </c>
+      <c r="G136" s="5">
+        <v>43995</v>
+      </c>
+      <c r="H136">
+        <v>21181</v>
+      </c>
+      <c r="I136">
+        <v>14832</v>
+      </c>
+      <c r="J136" s="5">
+        <v>43995</v>
+      </c>
+      <c r="K136">
+        <v>383</v>
+      </c>
+      <c r="L136">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12">
+      <c r="A137" s="5">
+        <v>43996</v>
+      </c>
+      <c r="B137">
+        <v>79452</v>
+      </c>
+      <c r="C137">
+        <v>73221</v>
+      </c>
+      <c r="D137" s="5">
+        <v>43996</v>
+      </c>
+      <c r="E137">
+        <v>36198</v>
+      </c>
+      <c r="F137">
+        <v>18780</v>
+      </c>
+      <c r="G137" s="5">
+        <v>43996</v>
+      </c>
+      <c r="H137">
+        <v>19302</v>
+      </c>
+      <c r="I137">
+        <v>15083</v>
+      </c>
+      <c r="J137" s="5">
+        <v>43996</v>
+      </c>
+      <c r="K137">
+        <v>345</v>
+      </c>
+      <c r="L137">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" s="5">
+        <v>43997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix the bug of chinese date in excel
</commit_message>
<xml_diff>
--- a/handleData/data/regions.xlsx
+++ b/handleData/data/regions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13030" windowHeight="7290" firstSheet="1" activeTab="4"/>
+    <workbookView windowWidth="16850" windowHeight="7740" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="全球" sheetId="2" r:id="rId1"/>
@@ -86,14 +86,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  <numFmts count="6">
+    <numFmt numFmtId="176" formatCode="m/d;@"/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="m/d;@"/>
+    <numFmt numFmtId="177" formatCode="0_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,10 +125,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF666666"/>
+      <name val="Arial"/>
+      <charset val="204"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -137,16 +159,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -160,25 +197,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -190,8 +221,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -213,39 +259,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -259,22 +275,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -283,7 +291,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -295,85 +369,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -391,31 +387,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -433,42 +465,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -477,13 +491,52 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -503,59 +556,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -574,6 +581,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -582,10 +607,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -594,137 +619,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -746,7 +771,13 @@
     <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1366,10 +1397,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C138"/>
+  <dimension ref="A1:C152"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="D139" sqref="D139"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="D157" sqref="D157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -2653,11 +2684,11 @@
       <c r="A118" s="5">
         <v>43977</v>
       </c>
-      <c r="B118" s="7">
+      <c r="B118" s="9">
         <f>([1]总计!B118-[1]总计!B117)</f>
         <v>83417</v>
       </c>
-      <c r="C118" s="7">
+      <c r="C118" s="9">
         <f>([1]总计!F118-[1]总计!F117)</f>
         <v>62590</v>
       </c>
@@ -2666,11 +2697,11 @@
       <c r="A119" s="5">
         <v>43978</v>
       </c>
-      <c r="B119" s="7">
+      <c r="B119" s="9">
         <f>([1]总计!B119-[1]总计!B118)</f>
         <v>82844</v>
       </c>
-      <c r="C119" s="7">
+      <c r="C119" s="9">
         <f>([1]总计!F119-[1]总计!F118)</f>
         <v>64065</v>
       </c>
@@ -2679,11 +2710,11 @@
       <c r="A120" s="5">
         <v>43979</v>
       </c>
-      <c r="B120" s="7">
+      <c r="B120" s="9">
         <f>([1]总计!B120-[1]总计!B119)</f>
         <v>110750</v>
       </c>
-      <c r="C120" s="7">
+      <c r="C120" s="9">
         <f>([1]总计!F120-[1]总计!F119)</f>
         <v>59543</v>
       </c>
@@ -2692,11 +2723,11 @@
       <c r="A121" s="5">
         <v>43980</v>
       </c>
-      <c r="B121" s="7">
+      <c r="B121" s="9">
         <f>([1]总计!B121-[1]总计!B120)</f>
         <v>105554</v>
       </c>
-      <c r="C121" s="7">
+      <c r="C121" s="9">
         <f>([1]总计!F121-[1]总计!F120)</f>
         <v>93127</v>
       </c>
@@ -2705,11 +2736,11 @@
       <c r="A122" s="5">
         <v>43981</v>
       </c>
-      <c r="B122" s="7">
+      <c r="B122" s="9">
         <f>([1]总计!B122-[1]总计!B121)</f>
         <v>124610</v>
       </c>
-      <c r="C122" s="7">
+      <c r="C122" s="9">
         <f>([1]总计!F122-[1]总计!F121)</f>
         <v>80053</v>
       </c>
@@ -2718,11 +2749,11 @@
       <c r="A123" s="5">
         <v>43982</v>
       </c>
-      <c r="B123" s="7">
+      <c r="B123" s="9">
         <f>([1]总计!B123-[1]总计!B122)</f>
         <v>121855</v>
       </c>
-      <c r="C123" s="7">
+      <c r="C123" s="9">
         <f>([1]总计!F123-[1]总计!F122)</f>
         <v>62310</v>
       </c>
@@ -2881,9 +2912,163 @@
         <v>108403</v>
       </c>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:3">
       <c r="A138" s="5">
         <v>43997</v>
+      </c>
+      <c r="B138">
+        <v>127609</v>
+      </c>
+      <c r="C138">
+        <v>79284</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="5">
+        <v>43998</v>
+      </c>
+      <c r="B139">
+        <v>136142</v>
+      </c>
+      <c r="C139">
+        <v>117720</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="5">
+        <v>43999</v>
+      </c>
+      <c r="B140">
+        <v>115885</v>
+      </c>
+      <c r="C140">
+        <v>75916</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="5">
+        <v>44000</v>
+      </c>
+      <c r="B141">
+        <v>150813</v>
+      </c>
+      <c r="C141">
+        <v>86498</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="5">
+        <v>44001</v>
+      </c>
+      <c r="B142">
+        <v>172581</v>
+      </c>
+      <c r="C142">
+        <v>125697</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="5">
+        <v>44002</v>
+      </c>
+      <c r="B143">
+        <v>182369</v>
+      </c>
+      <c r="C143">
+        <v>114032</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="5">
+        <v>44003</v>
+      </c>
+      <c r="B144">
+        <v>160460</v>
+      </c>
+      <c r="C144">
+        <v>109300</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" s="5">
+        <v>44004</v>
+      </c>
+      <c r="B145">
+        <v>131916</v>
+      </c>
+      <c r="C145">
+        <v>68670</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" s="5">
+        <v>44005</v>
+      </c>
+      <c r="B146">
+        <v>139735</v>
+      </c>
+      <c r="C146">
+        <v>107875</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="5">
+        <v>44006</v>
+      </c>
+      <c r="B147">
+        <v>163068</v>
+      </c>
+      <c r="C147">
+        <v>102322</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" s="5">
+        <v>44007</v>
+      </c>
+      <c r="B148">
+        <v>173105</v>
+      </c>
+      <c r="C148">
+        <v>156953</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" s="5">
+        <v>44008</v>
+      </c>
+      <c r="B149">
+        <v>177906</v>
+      </c>
+      <c r="C149">
+        <v>86682</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" s="5">
+        <v>44009</v>
+      </c>
+      <c r="B150">
+        <v>196597</v>
+      </c>
+      <c r="C150">
+        <v>70851</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" s="5">
+        <v>44010</v>
+      </c>
+      <c r="B151">
+        <v>176836</v>
+      </c>
+      <c r="C151">
+        <v>108666</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" s="5">
+        <v>44011</v>
       </c>
     </row>
   </sheetData>
@@ -2895,10 +3080,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C138"/>
+  <dimension ref="A1:C152"/>
   <sheetViews>
-    <sheetView topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="H129" sqref="H129"/>
+    <sheetView topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="F149" sqref="F149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -4398,9 +4583,163 @@
         <v>4058</v>
       </c>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:3">
       <c r="A138" s="5">
         <v>43997</v>
+      </c>
+      <c r="B138">
+        <v>8043</v>
+      </c>
+      <c r="C138">
+        <v>3296</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="5">
+        <v>43998</v>
+      </c>
+      <c r="B139">
+        <v>10968</v>
+      </c>
+      <c r="C139">
+        <v>4542</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="5">
+        <v>43999</v>
+      </c>
+      <c r="B140">
+        <v>3711</v>
+      </c>
+      <c r="C140">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="5">
+        <v>44000</v>
+      </c>
+      <c r="B141">
+        <v>11204</v>
+      </c>
+      <c r="C141">
+        <v>6412</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="5">
+        <v>44001</v>
+      </c>
+      <c r="B142">
+        <v>8391</v>
+      </c>
+      <c r="C142">
+        <v>2946</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="5">
+        <v>44002</v>
+      </c>
+      <c r="B143">
+        <v>10402</v>
+      </c>
+      <c r="C143">
+        <v>7066</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="5">
+        <v>44003</v>
+      </c>
+      <c r="B144">
+        <v>10087</v>
+      </c>
+      <c r="C144">
+        <v>9842</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" s="5">
+        <v>44004</v>
+      </c>
+      <c r="B145">
+        <v>10222</v>
+      </c>
+      <c r="C145">
+        <v>3974</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" s="5">
+        <v>44005</v>
+      </c>
+      <c r="B146">
+        <v>8712</v>
+      </c>
+      <c r="C146">
+        <v>3935</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="5">
+        <v>44006</v>
+      </c>
+      <c r="B147">
+        <v>9089</v>
+      </c>
+      <c r="C147">
+        <v>3910</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" s="5">
+        <v>44007</v>
+      </c>
+      <c r="B148">
+        <v>11598</v>
+      </c>
+      <c r="C148">
+        <v>6381</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" s="5">
+        <v>44008</v>
+      </c>
+      <c r="B149">
+        <v>11299</v>
+      </c>
+      <c r="C149">
+        <v>5079</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" s="5">
+        <v>44009</v>
+      </c>
+      <c r="B150">
+        <v>11766</v>
+      </c>
+      <c r="C150">
+        <v>6790</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" s="5">
+        <v>44010</v>
+      </c>
+      <c r="B151">
+        <v>12631</v>
+      </c>
+      <c r="C151">
+        <v>5653</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" s="5">
+        <v>44011</v>
       </c>
     </row>
   </sheetData>
@@ -4412,10 +4751,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C138"/>
+  <dimension ref="A1:C152"/>
   <sheetViews>
-    <sheetView topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="B132" sqref="B132:C137"/>
+    <sheetView topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="D149" sqref="D149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -5918,9 +6257,163 @@
         <v>24783</v>
       </c>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:3">
       <c r="A138" s="5">
         <v>43997</v>
+      </c>
+      <c r="B138">
+        <v>30056</v>
+      </c>
+      <c r="C138">
+        <v>16768</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="5">
+        <v>43998</v>
+      </c>
+      <c r="B139">
+        <v>26927</v>
+      </c>
+      <c r="C139">
+        <v>19009</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="5">
+        <v>43999</v>
+      </c>
+      <c r="B140">
+        <v>27082</v>
+      </c>
+      <c r="C140">
+        <v>21835</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="5">
+        <v>44000</v>
+      </c>
+      <c r="B141">
+        <v>30106</v>
+      </c>
+      <c r="C141">
+        <v>21033</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="5">
+        <v>44001</v>
+      </c>
+      <c r="B142">
+        <v>30869</v>
+      </c>
+      <c r="C142">
+        <v>24074</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="5">
+        <v>44002</v>
+      </c>
+      <c r="B143">
+        <v>30952</v>
+      </c>
+      <c r="C143">
+        <v>23449</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="5">
+        <v>44003</v>
+      </c>
+      <c r="B144">
+        <v>34362</v>
+      </c>
+      <c r="C144">
+        <v>28364</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" s="5">
+        <v>44004</v>
+      </c>
+      <c r="B145">
+        <v>31056</v>
+      </c>
+      <c r="C145">
+        <v>20475</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" s="5">
+        <v>44005</v>
+      </c>
+      <c r="B146" s="7">
+        <v>28929</v>
+      </c>
+      <c r="C146" s="8">
+        <v>20599</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="5">
+        <v>44006</v>
+      </c>
+      <c r="B147" s="7">
+        <v>30921</v>
+      </c>
+      <c r="C147" s="8">
+        <v>26269</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" s="5">
+        <v>44007</v>
+      </c>
+      <c r="B148" s="7">
+        <v>31331</v>
+      </c>
+      <c r="C148" s="8">
+        <v>31861</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" s="5">
+        <v>44008</v>
+      </c>
+      <c r="B149" s="7">
+        <v>33189</v>
+      </c>
+      <c r="C149" s="8">
+        <v>26164</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" s="5">
+        <v>44009</v>
+      </c>
+      <c r="B150" s="7">
+        <v>31909</v>
+      </c>
+      <c r="C150" s="8">
+        <v>24359</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" s="5">
+        <v>44010</v>
+      </c>
+      <c r="B151" s="7">
+        <v>34091</v>
+      </c>
+      <c r="C151" s="8">
+        <v>28177</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" s="5">
+        <v>44011</v>
       </c>
     </row>
   </sheetData>
@@ -5932,10 +6425,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C138"/>
+  <dimension ref="A1:C152"/>
   <sheetViews>
-    <sheetView topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="B132" sqref="B132:C137"/>
+    <sheetView topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="E148" sqref="E148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -7435,9 +7928,163 @@
         <v>38704</v>
       </c>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:3">
       <c r="A138" s="5">
         <v>43997</v>
+      </c>
+      <c r="B138">
+        <v>50933</v>
+      </c>
+      <c r="C138">
+        <v>31468</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="5">
+        <v>43998</v>
+      </c>
+      <c r="B139">
+        <v>47605</v>
+      </c>
+      <c r="C139">
+        <v>33391</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="5">
+        <v>43999</v>
+      </c>
+      <c r="B140">
+        <v>48291</v>
+      </c>
+      <c r="C140">
+        <v>53629</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="5">
+        <v>44000</v>
+      </c>
+      <c r="B141">
+        <v>52833</v>
+      </c>
+      <c r="C141">
+        <v>37500</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="5">
+        <v>44001</v>
+      </c>
+      <c r="B142">
+        <v>52871</v>
+      </c>
+      <c r="C142">
+        <v>41577</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="5">
+        <v>44002</v>
+      </c>
+      <c r="B143">
+        <v>52097</v>
+      </c>
+      <c r="C143">
+        <v>41845</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="5">
+        <v>44003</v>
+      </c>
+      <c r="B144">
+        <v>55048</v>
+      </c>
+      <c r="C144">
+        <v>45533</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" s="5">
+        <v>44004</v>
+      </c>
+      <c r="B145">
+        <v>50473</v>
+      </c>
+      <c r="C145">
+        <v>36064</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" s="5">
+        <v>44005</v>
+      </c>
+      <c r="B146">
+        <v>49891</v>
+      </c>
+      <c r="C146">
+        <v>38018</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="5">
+        <v>44006</v>
+      </c>
+      <c r="B147">
+        <v>51783</v>
+      </c>
+      <c r="C147">
+        <v>44613</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" s="5">
+        <v>44007</v>
+      </c>
+      <c r="B148">
+        <v>53909</v>
+      </c>
+      <c r="C148">
+        <v>51310</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" s="5">
+        <v>44008</v>
+      </c>
+      <c r="B149">
+        <v>56903</v>
+      </c>
+      <c r="C149">
+        <v>47320</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" s="5">
+        <v>44009</v>
+      </c>
+      <c r="B150">
+        <v>55416</v>
+      </c>
+      <c r="C150">
+        <v>42713</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" s="5">
+        <v>44010</v>
+      </c>
+      <c r="B151">
+        <v>56522</v>
+      </c>
+      <c r="C151">
+        <v>45538</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" s="5">
+        <v>44011</v>
       </c>
     </row>
   </sheetData>
@@ -7449,10 +8096,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L138"/>
+  <dimension ref="A1:L152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="E93" sqref="E93:E137"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="E151" sqref="E151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14"/>
@@ -12637,9 +13284,541 @@
         <v>205</v>
       </c>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:12">
       <c r="A138" s="5">
         <v>43997</v>
+      </c>
+      <c r="B138">
+        <v>77392</v>
+      </c>
+      <c r="C138">
+        <v>48160</v>
+      </c>
+      <c r="D138" s="5">
+        <v>43997</v>
+      </c>
+      <c r="E138">
+        <v>29521</v>
+      </c>
+      <c r="F138">
+        <v>17749</v>
+      </c>
+      <c r="G138" s="5">
+        <v>43997</v>
+      </c>
+      <c r="H138">
+        <v>19584</v>
+      </c>
+      <c r="I138">
+        <v>12553</v>
+      </c>
+      <c r="J138" s="5">
+        <v>43997</v>
+      </c>
+      <c r="K138">
+        <v>298</v>
+      </c>
+      <c r="L138">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12">
+      <c r="A139" s="5">
+        <v>43998</v>
+      </c>
+      <c r="B139">
+        <v>81006</v>
+      </c>
+      <c r="C139">
+        <v>67520</v>
+      </c>
+      <c r="D139" s="5">
+        <v>43998</v>
+      </c>
+      <c r="E139">
+        <v>30864</v>
+      </c>
+      <c r="F139">
+        <v>35255</v>
+      </c>
+      <c r="G139" s="5">
+        <v>43998</v>
+      </c>
+      <c r="H139">
+        <v>21614</v>
+      </c>
+      <c r="I139">
+        <v>12801</v>
+      </c>
+      <c r="J139" s="5">
+        <v>43998</v>
+      </c>
+      <c r="K139">
+        <v>377</v>
+      </c>
+      <c r="L139">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12">
+      <c r="A140" s="5">
+        <v>43999</v>
+      </c>
+      <c r="B140">
+        <v>65924</v>
+      </c>
+      <c r="C140">
+        <v>42537</v>
+      </c>
+      <c r="D140" s="5">
+        <v>43999</v>
+      </c>
+      <c r="E140">
+        <v>29421</v>
+      </c>
+      <c r="F140">
+        <v>15032</v>
+      </c>
+      <c r="G140" s="5">
+        <v>43999</v>
+      </c>
+      <c r="H140">
+        <v>18441</v>
+      </c>
+      <c r="I140">
+        <v>16747</v>
+      </c>
+      <c r="J140" s="5">
+        <v>43999</v>
+      </c>
+      <c r="K140">
+        <v>437</v>
+      </c>
+      <c r="L140">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12">
+      <c r="A141" s="5">
+        <v>44000</v>
+      </c>
+      <c r="B141">
+        <v>89104</v>
+      </c>
+      <c r="C141">
+        <v>48016</v>
+      </c>
+      <c r="D141" s="5">
+        <v>44000</v>
+      </c>
+      <c r="E141">
+        <v>39555</v>
+      </c>
+      <c r="F141">
+        <v>19339</v>
+      </c>
+      <c r="G141" s="5">
+        <v>44000</v>
+      </c>
+      <c r="H141">
+        <v>19850</v>
+      </c>
+      <c r="I141">
+        <v>17821</v>
+      </c>
+      <c r="J141" s="5">
+        <v>44000</v>
+      </c>
+      <c r="K141">
+        <v>547</v>
+      </c>
+      <c r="L141">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12">
+      <c r="A142" s="5">
+        <v>44001</v>
+      </c>
+      <c r="B142">
+        <v>113783</v>
+      </c>
+      <c r="C142">
+        <v>85843</v>
+      </c>
+      <c r="D142" s="5">
+        <v>44001</v>
+      </c>
+      <c r="E142">
+        <v>36907</v>
+      </c>
+      <c r="F142">
+        <v>20666</v>
+      </c>
+      <c r="G142" s="5">
+        <v>44001</v>
+      </c>
+      <c r="H142">
+        <v>20097</v>
+      </c>
+      <c r="I142">
+        <v>17426</v>
+      </c>
+      <c r="J142" s="5">
+        <v>44001</v>
+      </c>
+      <c r="K142">
+        <v>505</v>
+      </c>
+      <c r="L142">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12">
+      <c r="A143" s="5">
+        <v>44002</v>
+      </c>
+      <c r="B143">
+        <v>114197</v>
+      </c>
+      <c r="C143">
+        <v>56918</v>
+      </c>
+      <c r="D143" s="5">
+        <v>44002</v>
+      </c>
+      <c r="E143">
+        <v>44983</v>
+      </c>
+      <c r="F143">
+        <v>35702</v>
+      </c>
+      <c r="G143" s="5">
+        <v>44002</v>
+      </c>
+      <c r="H143">
+        <v>20770</v>
+      </c>
+      <c r="I143">
+        <v>20126</v>
+      </c>
+      <c r="J143" s="5">
+        <v>44002</v>
+      </c>
+      <c r="K143">
+        <v>673</v>
+      </c>
+      <c r="L143">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12">
+      <c r="A144" s="5">
+        <v>44003</v>
+      </c>
+      <c r="B144">
+        <v>96356</v>
+      </c>
+      <c r="C144">
+        <v>64814</v>
+      </c>
+      <c r="D144" s="5">
+        <v>44003</v>
+      </c>
+      <c r="E144">
+        <v>42014</v>
+      </c>
+      <c r="F144">
+        <v>18463</v>
+      </c>
+      <c r="G144" s="5">
+        <v>44003</v>
+      </c>
+      <c r="H144">
+        <v>19624</v>
+      </c>
+      <c r="I144">
+        <v>24951</v>
+      </c>
+      <c r="J144" s="5">
+        <v>44003</v>
+      </c>
+      <c r="K144">
+        <v>666</v>
+      </c>
+      <c r="L144">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12">
+      <c r="A145" s="5">
+        <v>44004</v>
+      </c>
+      <c r="B145">
+        <v>75199</v>
+      </c>
+      <c r="C145">
+        <v>36491</v>
+      </c>
+      <c r="D145" s="5">
+        <v>44004</v>
+      </c>
+      <c r="E145">
+        <v>34701</v>
+      </c>
+      <c r="F145">
+        <v>17728</v>
+      </c>
+      <c r="G145" s="5">
+        <v>44004</v>
+      </c>
+      <c r="H145">
+        <v>19975</v>
+      </c>
+      <c r="I145">
+        <v>12725</v>
+      </c>
+      <c r="J145" s="5">
+        <v>44004</v>
+      </c>
+      <c r="K145">
+        <v>404</v>
+      </c>
+      <c r="L145">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12">
+      <c r="A146" s="5">
+        <v>44005</v>
+      </c>
+      <c r="B146">
+        <v>77097</v>
+      </c>
+      <c r="C146">
+        <v>75505</v>
+      </c>
+      <c r="D146" s="5">
+        <v>44005</v>
+      </c>
+      <c r="E146">
+        <v>43151</v>
+      </c>
+      <c r="F146">
+        <v>18866</v>
+      </c>
+      <c r="G146" s="5">
+        <v>44005</v>
+      </c>
+      <c r="H146">
+        <v>17565</v>
+      </c>
+      <c r="I146">
+        <v>12048</v>
+      </c>
+      <c r="J146" s="5">
+        <v>44005</v>
+      </c>
+      <c r="K146">
+        <v>646</v>
+      </c>
+      <c r="L146">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12">
+      <c r="A147" s="5">
+        <v>44006</v>
+      </c>
+      <c r="B147">
+        <v>96203</v>
+      </c>
+      <c r="C147">
+        <v>52780</v>
+      </c>
+      <c r="D147" s="5">
+        <v>44006</v>
+      </c>
+      <c r="E147">
+        <v>45758</v>
+      </c>
+      <c r="F147">
+        <v>25939</v>
+      </c>
+      <c r="G147" s="5">
+        <v>44006</v>
+      </c>
+      <c r="H147">
+        <v>19063</v>
+      </c>
+      <c r="I147">
+        <v>21590</v>
+      </c>
+      <c r="J147" s="5">
+        <v>44006</v>
+      </c>
+      <c r="K147">
+        <v>837</v>
+      </c>
+      <c r="L147">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12">
+      <c r="A148" s="5">
+        <v>44007</v>
+      </c>
+      <c r="B148">
+        <v>104898</v>
+      </c>
+      <c r="C148">
+        <v>99900</v>
+      </c>
+      <c r="D148" s="5">
+        <v>44007</v>
+      </c>
+      <c r="E148">
+        <v>46630</v>
+      </c>
+      <c r="F148">
+        <v>32740</v>
+      </c>
+      <c r="G148" s="5">
+        <v>44007</v>
+      </c>
+      <c r="H148">
+        <v>17978</v>
+      </c>
+      <c r="I148">
+        <v>22757</v>
+      </c>
+      <c r="J148" s="5">
+        <v>44007</v>
+      </c>
+      <c r="K148">
+        <v>944</v>
+      </c>
+      <c r="L148">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12">
+      <c r="A149" s="5">
+        <v>44008</v>
+      </c>
+      <c r="B149">
+        <v>106186</v>
+      </c>
+      <c r="C149">
+        <v>46161</v>
+      </c>
+      <c r="D149" s="5">
+        <v>44008</v>
+      </c>
+      <c r="E149">
+        <v>49710</v>
+      </c>
+      <c r="F149">
+        <v>21331</v>
+      </c>
+      <c r="G149" s="5">
+        <v>44008</v>
+      </c>
+      <c r="H149">
+        <v>19776</v>
+      </c>
+      <c r="I149">
+        <v>18091</v>
+      </c>
+      <c r="J149" s="5">
+        <v>44008</v>
+      </c>
+      <c r="K149">
+        <v>696</v>
+      </c>
+      <c r="L149">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12">
+      <c r="A150" s="5">
+        <v>44009</v>
+      </c>
+      <c r="B150">
+        <v>112189</v>
+      </c>
+      <c r="C150">
+        <v>31117</v>
+      </c>
+      <c r="D150" s="5">
+        <v>44009</v>
+      </c>
+      <c r="E150">
+        <v>61560</v>
+      </c>
+      <c r="F150">
+        <v>19910</v>
+      </c>
+      <c r="G150" s="5">
+        <v>44009</v>
+      </c>
+      <c r="H150">
+        <v>19598</v>
+      </c>
+      <c r="I150">
+        <v>17091</v>
+      </c>
+      <c r="J150" s="5">
+        <v>44009</v>
+      </c>
+      <c r="K150">
+        <v>925</v>
+      </c>
+      <c r="L150">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12">
+      <c r="A151" s="5">
+        <v>44010</v>
+      </c>
+      <c r="B151">
+        <v>101482</v>
+      </c>
+      <c r="C151">
+        <v>63743</v>
+      </c>
+      <c r="D151" s="5">
+        <v>44010</v>
+      </c>
+      <c r="E151">
+        <v>52081</v>
+      </c>
+      <c r="F151">
+        <v>26012</v>
+      </c>
+      <c r="G151" s="5">
+        <v>44010</v>
+      </c>
+      <c r="H151">
+        <v>19463</v>
+      </c>
+      <c r="I151">
+        <v>17182</v>
+      </c>
+      <c r="J151" s="5">
+        <v>44010</v>
+      </c>
+      <c r="K151">
+        <v>1293</v>
+      </c>
+      <c r="L151">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" s="5">
+        <v>44011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change weekly growth to the new algorith
</commit_message>
<xml_diff>
--- a/handleData/data/regions.xlsx
+++ b/handleData/data/regions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16850" windowHeight="7740" activeTab="4"/>
+    <workbookView windowWidth="12950" windowHeight="7290"/>
   </bookViews>
   <sheets>
     <sheet name="全球" sheetId="2" r:id="rId1"/>
@@ -87,12 +87,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="m/d;@"/>
+    <numFmt numFmtId="176" formatCode="0_ "/>
+    <numFmt numFmtId="177" formatCode="m/d;@"/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="0_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -139,98 +139,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -244,16 +153,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -269,7 +208,53 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -277,6 +262,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -297,19 +297,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -321,7 +315,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -333,49 +345,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -393,7 +363,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -405,43 +393,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -459,7 +429,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -471,13 +459,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -502,11 +502,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -526,6 +550,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -541,17 +580,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -566,39 +599,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -607,10 +607,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -619,133 +619,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -765,13 +765,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1397,10 +1397,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C152"/>
+  <dimension ref="A1:C159"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="D157" sqref="D157"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="A152" sqref="A152:A159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -3066,9 +3066,86 @@
         <v>108666</v>
       </c>
     </row>
-    <row r="152" spans="1:1">
+    <row r="152" spans="1:3">
       <c r="A152" s="5">
         <v>44011</v>
+      </c>
+      <c r="B152">
+        <v>171824</v>
+      </c>
+      <c r="C152">
+        <v>118918</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" s="5">
+        <v>44012</v>
+      </c>
+      <c r="B153">
+        <v>156100</v>
+      </c>
+      <c r="C153">
+        <v>74458</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154" s="5">
+        <v>44013</v>
+      </c>
+      <c r="B154">
+        <v>172390</v>
+      </c>
+      <c r="C154">
+        <v>121093</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" s="5">
+        <v>44014</v>
+      </c>
+      <c r="B155">
+        <v>199089</v>
+      </c>
+      <c r="C155">
+        <v>133961</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" s="5">
+        <v>44015</v>
+      </c>
+      <c r="B156">
+        <v>231043</v>
+      </c>
+      <c r="C156">
+        <v>251613</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" s="5">
+        <v>44016</v>
+      </c>
+      <c r="B157">
+        <v>177695</v>
+      </c>
+      <c r="C157">
+        <v>104113</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" s="5">
+        <v>44017</v>
+      </c>
+      <c r="B158">
+        <v>185135</v>
+      </c>
+      <c r="C158">
+        <v>190805</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" s="5">
+        <v>44018</v>
       </c>
     </row>
   </sheetData>
@@ -3080,10 +3157,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C152"/>
+  <dimension ref="A1:C161"/>
   <sheetViews>
-    <sheetView topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="F149" sqref="F149"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="F151" sqref="F151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -4737,9 +4814,96 @@
         <v>5653</v>
       </c>
     </row>
-    <row r="152" spans="1:1">
+    <row r="152" spans="1:3">
       <c r="A152" s="5">
         <v>44011</v>
+      </c>
+      <c r="B152">
+        <v>10948</v>
+      </c>
+      <c r="C152">
+        <v>4262</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" s="5">
+        <v>44012</v>
+      </c>
+      <c r="B153">
+        <v>10639</v>
+      </c>
+      <c r="C153">
+        <v>4146</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154" s="5">
+        <v>44013</v>
+      </c>
+      <c r="B154">
+        <v>11949</v>
+      </c>
+      <c r="C154">
+        <v>5922</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" s="5">
+        <v>44014</v>
+      </c>
+      <c r="B155">
+        <v>11995</v>
+      </c>
+      <c r="C155">
+        <v>4454</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" s="5">
+        <v>44015</v>
+      </c>
+      <c r="B156">
+        <v>14402</v>
+      </c>
+      <c r="C156">
+        <v>9432</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" s="5">
+        <v>44016</v>
+      </c>
+      <c r="B157">
+        <v>14741</v>
+      </c>
+      <c r="C157">
+        <v>7524</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" s="5">
+        <v>44017</v>
+      </c>
+      <c r="B158">
+        <v>16571</v>
+      </c>
+      <c r="C158">
+        <v>7680</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" s="5">
+        <v>44018</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" s="5">
+        <v>44019</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" s="5">
+        <v>44020</v>
       </c>
     </row>
   </sheetData>
@@ -4751,10 +4915,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C152"/>
+  <dimension ref="A1:C160"/>
   <sheetViews>
-    <sheetView topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="D149" sqref="D149"/>
+    <sheetView topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="E160" sqref="E160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -6411,9 +6575,91 @@
         <v>28177</v>
       </c>
     </row>
-    <row r="152" spans="1:1">
+    <row r="152" spans="1:3">
       <c r="A152" s="5">
         <v>44011</v>
+      </c>
+      <c r="B152">
+        <v>34142</v>
+      </c>
+      <c r="C152">
+        <v>26812</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" s="5">
+        <v>44012</v>
+      </c>
+      <c r="B153">
+        <v>32475</v>
+      </c>
+      <c r="C153">
+        <v>23711</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154" s="5">
+        <v>44013</v>
+      </c>
+      <c r="B154">
+        <v>31684</v>
+      </c>
+      <c r="C154">
+        <v>26790</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" s="5">
+        <v>44014</v>
+      </c>
+      <c r="B155">
+        <v>34551</v>
+      </c>
+      <c r="C155">
+        <v>29894</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" s="5">
+        <v>44015</v>
+      </c>
+      <c r="B156">
+        <v>56715</v>
+      </c>
+      <c r="C156">
+        <v>44458</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" s="5">
+        <v>44016</v>
+      </c>
+      <c r="B157">
+        <v>39691</v>
+      </c>
+      <c r="C157">
+        <v>36738</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" s="5">
+        <v>44017</v>
+      </c>
+      <c r="B158">
+        <v>39965</v>
+      </c>
+      <c r="C158">
+        <v>38818</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" s="5">
+        <v>44018</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" s="5">
+        <v>44019</v>
       </c>
     </row>
   </sheetData>
@@ -6425,10 +6671,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C152"/>
+  <dimension ref="A1:C159"/>
   <sheetViews>
-    <sheetView topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="E148" sqref="E148"/>
+    <sheetView topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="A152" sqref="A152:A159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -8082,9 +8328,86 @@
         <v>45538</v>
       </c>
     </row>
-    <row r="152" spans="1:1">
+    <row r="152" spans="1:3">
       <c r="A152" s="5">
         <v>44011</v>
+      </c>
+      <c r="B152" s="7">
+        <v>56407</v>
+      </c>
+      <c r="C152" s="8">
+        <v>44039</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" s="5">
+        <v>44012</v>
+      </c>
+      <c r="B153" s="7">
+        <v>54454</v>
+      </c>
+      <c r="C153" s="8">
+        <v>41161</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154" s="5">
+        <v>44013</v>
+      </c>
+      <c r="B154" s="7">
+        <v>54544</v>
+      </c>
+      <c r="C154" s="8">
+        <v>45735</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" s="5">
+        <v>44014</v>
+      </c>
+      <c r="B155" s="7">
+        <v>57520</v>
+      </c>
+      <c r="C155" s="8">
+        <v>50851</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" s="5">
+        <v>44015</v>
+      </c>
+      <c r="B156" s="7">
+        <v>79681</v>
+      </c>
+      <c r="C156" s="8">
+        <v>68801</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" s="5">
+        <v>44016</v>
+      </c>
+      <c r="B157" s="7">
+        <v>63868</v>
+      </c>
+      <c r="C157" s="8">
+        <v>56748</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" s="5">
+        <v>44017</v>
+      </c>
+      <c r="B158" s="7">
+        <v>63216</v>
+      </c>
+      <c r="C158" s="8">
+        <v>58138</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" s="5">
+        <v>44018</v>
       </c>
     </row>
   </sheetData>
@@ -8096,10 +8419,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L152"/>
+  <dimension ref="A1:L159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="E151" sqref="E151"/>
+    <sheetView topLeftCell="A140" workbookViewId="0">
+      <selection activeCell="N154" sqref="N154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14"/>
@@ -13816,9 +14139,275 @@
         <v>471</v>
       </c>
     </row>
-    <row r="152" spans="1:1">
+    <row r="152" spans="1:12">
       <c r="A152" s="5">
         <v>44011</v>
+      </c>
+      <c r="B152">
+        <v>102479</v>
+      </c>
+      <c r="C152">
+        <v>86681</v>
+      </c>
+      <c r="D152" s="5">
+        <v>44011</v>
+      </c>
+      <c r="E152">
+        <v>48270</v>
+      </c>
+      <c r="F152">
+        <v>17500</v>
+      </c>
+      <c r="G152" s="5">
+        <v>44011</v>
+      </c>
+      <c r="H152">
+        <v>18091</v>
+      </c>
+      <c r="I152">
+        <v>13494</v>
+      </c>
+      <c r="J152" s="5">
+        <v>44011</v>
+      </c>
+      <c r="K152">
+        <v>854</v>
+      </c>
+      <c r="L152">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12">
+      <c r="A153" s="5">
+        <v>44012</v>
+      </c>
+      <c r="B153">
+        <v>80560</v>
+      </c>
+      <c r="C153">
+        <v>40738</v>
+      </c>
+      <c r="D153" s="5">
+        <v>44012</v>
+      </c>
+      <c r="E153">
+        <v>52708</v>
+      </c>
+      <c r="F153">
+        <v>20496</v>
+      </c>
+      <c r="G153" s="5">
+        <v>44012</v>
+      </c>
+      <c r="H153">
+        <v>19977</v>
+      </c>
+      <c r="I153">
+        <v>11466</v>
+      </c>
+      <c r="J153" s="5">
+        <v>44012</v>
+      </c>
+      <c r="K153">
+        <v>1220</v>
+      </c>
+      <c r="L153">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12">
+      <c r="A154" s="5">
+        <v>44013</v>
+      </c>
+      <c r="B154">
+        <v>92808</v>
+      </c>
+      <c r="C154">
+        <v>67885</v>
+      </c>
+      <c r="D154" s="5">
+        <v>44013</v>
+      </c>
+      <c r="E154">
+        <v>55973</v>
+      </c>
+      <c r="F154">
+        <v>32942</v>
+      </c>
+      <c r="G154" s="5">
+        <v>44013</v>
+      </c>
+      <c r="H154">
+        <v>19916</v>
+      </c>
+      <c r="I154">
+        <v>17940</v>
+      </c>
+      <c r="J154" s="5">
+        <v>44013</v>
+      </c>
+      <c r="K154">
+        <v>1465</v>
+      </c>
+      <c r="L154">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12">
+      <c r="A155" s="5">
+        <v>44014</v>
+      </c>
+      <c r="B155">
+        <v>116226</v>
+      </c>
+      <c r="C155">
+        <v>81702</v>
+      </c>
+      <c r="D155" s="5">
+        <v>44014</v>
+      </c>
+      <c r="E155">
+        <v>61053</v>
+      </c>
+      <c r="F155">
+        <v>34031</v>
+      </c>
+      <c r="G155" s="5">
+        <v>44014</v>
+      </c>
+      <c r="H155">
+        <v>17538</v>
+      </c>
+      <c r="I155">
+        <v>17938</v>
+      </c>
+      <c r="J155" s="5">
+        <v>44014</v>
+      </c>
+      <c r="K155">
+        <v>1911</v>
+      </c>
+      <c r="L155">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12">
+      <c r="A156" s="5">
+        <v>44015</v>
+      </c>
+      <c r="B156">
+        <v>138934</v>
+      </c>
+      <c r="C156">
+        <v>196161</v>
+      </c>
+      <c r="D156" s="5">
+        <v>44015</v>
+      </c>
+      <c r="E156">
+        <v>68464</v>
+      </c>
+      <c r="F156">
+        <v>36710</v>
+      </c>
+      <c r="G156" s="5">
+        <v>44015</v>
+      </c>
+      <c r="H156">
+        <v>21114</v>
+      </c>
+      <c r="I156">
+        <v>17359</v>
+      </c>
+      <c r="J156" s="5">
+        <v>44015</v>
+      </c>
+      <c r="K156">
+        <v>1672</v>
+      </c>
+      <c r="L156">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12">
+      <c r="A157" s="5">
+        <v>44016</v>
+      </c>
+      <c r="B157">
+        <v>118744</v>
+      </c>
+      <c r="C157">
+        <v>56636</v>
+      </c>
+      <c r="D157" s="5">
+        <v>44016</v>
+      </c>
+      <c r="E157">
+        <v>64290</v>
+      </c>
+      <c r="F157">
+        <v>27480</v>
+      </c>
+      <c r="G157" s="5">
+        <v>44016</v>
+      </c>
+      <c r="H157">
+        <v>19649</v>
+      </c>
+      <c r="I157">
+        <v>17836</v>
+      </c>
+      <c r="J157" s="5">
+        <v>44016</v>
+      </c>
+      <c r="K157">
+        <v>2048</v>
+      </c>
+      <c r="L157">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12">
+      <c r="A158" s="5">
+        <v>44017</v>
+      </c>
+      <c r="B158">
+        <v>98359</v>
+      </c>
+      <c r="C158">
+        <v>114758</v>
+      </c>
+      <c r="D158" s="5">
+        <v>44017</v>
+      </c>
+      <c r="E158">
+        <v>58928</v>
+      </c>
+      <c r="F158">
+        <v>56347</v>
+      </c>
+      <c r="G158" s="5">
+        <v>44017</v>
+      </c>
+      <c r="H158">
+        <v>23279</v>
+      </c>
+      <c r="I158">
+        <v>18505</v>
+      </c>
+      <c r="J158" s="5">
+        <v>44017</v>
+      </c>
+      <c r="K158">
+        <v>2255</v>
+      </c>
+      <c r="L158">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" s="5">
+        <v>44018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gitignore xlsv/csv and avoid using newly number
</commit_message>
<xml_diff>
--- a/handleData/data/regions.xlsx
+++ b/handleData/data/regions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="12950" windowHeight="7290"/>
+    <workbookView windowWidth="16850" windowHeight="7290" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="全球" sheetId="2" r:id="rId1"/>
@@ -91,8 +91,8 @@
     <numFmt numFmtId="177" formatCode="m/d;@"/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -138,8 +138,107 @@
       <charset val="204"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -155,93 +254,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -254,7 +269,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -262,21 +277,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -297,7 +297,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -309,37 +399,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -351,67 +453,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -423,61 +471,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -502,6 +502,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -522,15 +533,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -583,19 +585,17 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -607,10 +607,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -619,133 +619,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1399,8 +1399,8 @@
   <sheetPr/>
   <dimension ref="A1:C159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="A152" sqref="A152:A159"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="A160" sqref="A160:D160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -3143,9 +3143,15 @@
         <v>190805</v>
       </c>
     </row>
-    <row r="159" spans="1:1">
+    <row r="159" spans="1:3">
       <c r="A159" s="5">
         <v>44018</v>
+      </c>
+      <c r="B159">
+        <v>184421</v>
+      </c>
+      <c r="C159">
+        <v>102765</v>
       </c>
     </row>
   </sheetData>
@@ -3159,8 +3165,8 @@
   <sheetPr/>
   <dimension ref="A1:C161"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="F151" sqref="F151"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="B159" sqref="B159:C159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -4891,9 +4897,15 @@
         <v>7680</v>
       </c>
     </row>
-    <row r="159" spans="1:1">
+    <row r="159" spans="1:3">
       <c r="A159" s="5">
         <v>44018</v>
+      </c>
+      <c r="B159">
+        <v>13838</v>
+      </c>
+      <c r="C159">
+        <v>5195</v>
       </c>
     </row>
     <row r="160" spans="1:1">
@@ -4918,7 +4930,7 @@
   <dimension ref="A1:C160"/>
   <sheetViews>
     <sheetView topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="E160" sqref="E160"/>
+      <selection activeCell="B159" sqref="B159:C159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -6652,9 +6664,15 @@
         <v>38818</v>
       </c>
     </row>
-    <row r="159" spans="1:1">
+    <row r="159" spans="1:3">
       <c r="A159" s="5">
         <v>44018</v>
+      </c>
+      <c r="B159">
+        <v>40538</v>
+      </c>
+      <c r="C159">
+        <v>27071</v>
       </c>
     </row>
     <row r="160" spans="1:1">
@@ -6674,7 +6692,7 @@
   <dimension ref="A1:C159"/>
   <sheetViews>
     <sheetView topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="A152" sqref="A152:A159"/>
+      <selection activeCell="G155" sqref="G155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -8405,9 +8423,15 @@
         <v>58138</v>
       </c>
     </row>
-    <row r="159" spans="1:1">
+    <row r="159" spans="1:3">
       <c r="A159" s="5">
         <v>44018</v>
+      </c>
+      <c r="B159">
+        <v>61587</v>
+      </c>
+      <c r="C159">
+        <v>44000</v>
       </c>
     </row>
   </sheetData>
@@ -8422,7 +8446,7 @@
   <dimension ref="A1:L159"/>
   <sheetViews>
     <sheetView topLeftCell="A140" workbookViewId="0">
-      <selection activeCell="N154" sqref="N154"/>
+      <selection activeCell="M159" sqref="M159:O159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14"/>
@@ -14405,9 +14429,42 @@
         <v>348</v>
       </c>
     </row>
-    <row r="159" spans="1:1">
+    <row r="159" spans="1:12">
       <c r="A159" s="5">
         <v>44018</v>
+      </c>
+      <c r="B159">
+        <v>101674</v>
+      </c>
+      <c r="C159">
+        <v>48255</v>
+      </c>
+      <c r="D159" s="5">
+        <v>44018</v>
+      </c>
+      <c r="E159">
+        <v>49673</v>
+      </c>
+      <c r="F159">
+        <v>34185</v>
+      </c>
+      <c r="G159" s="5">
+        <v>44018</v>
+      </c>
+      <c r="H159">
+        <v>20448</v>
+      </c>
+      <c r="I159">
+        <v>12049</v>
+      </c>
+      <c r="J159" s="5">
+        <v>44018</v>
+      </c>
+      <c r="K159">
+        <v>1829</v>
+      </c>
+      <c r="L159">
+        <v>367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>